<commit_message>
BTP done. Handing over.
</commit_message>
<xml_diff>
--- a/OutputData/After Normalization/Experienced data.xlsx
+++ b/OutputData/After Normalization/Experienced data.xlsx
@@ -827,24 +827,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="199262208"/>
-        <c:axId val="199263744"/>
+        <c:axId val="117137792"/>
+        <c:axId val="117139328"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="199262208"/>
+        <c:axId val="117137792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="199263744"/>
+        <c:crossAx val="117139328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="199263744"/>
+        <c:axId val="117139328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.8"/>
@@ -853,7 +853,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="199262208"/>
+        <c:crossAx val="117137792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -865,7 +865,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1268,11 +1268,11 @@
         </c:ser>
         <c:dropLines/>
         <c:marker val="1"/>
-        <c:axId val="216803968"/>
-        <c:axId val="193745280"/>
+        <c:axId val="117820032"/>
+        <c:axId val="117830784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="216803968"/>
+        <c:axId val="117820032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1280,14 +1280,14 @@
         <c:title/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="193745280"/>
+        <c:crossAx val="117830784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="193745280"/>
+        <c:axId val="117830784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1296,7 +1296,7 @@
         <c:title/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="216803968"/>
+        <c:crossAx val="117820032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1308,7 +1308,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1336,6 +1336,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln cmpd="dbl">
+              <a:prstDash val="dash"/>
+            </a:ln>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -1390,6 +1395,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:prstDash val="sysDash"/>
+            </a:ln>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -1444,6 +1454,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:prstDash val="sysDot"/>
+            </a:ln>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -1540,11 +1555,11 @@
         </c:ser>
         <c:dropLines/>
         <c:marker val="1"/>
-        <c:axId val="193839872"/>
-        <c:axId val="193841792"/>
+        <c:axId val="119149696"/>
+        <c:axId val="119151616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="193839872"/>
+        <c:axId val="119149696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1571,14 +1586,14 @@
         </c:title>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="193841792"/>
+        <c:crossAx val="119151616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="193841792"/>
+        <c:axId val="119151616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.8"/>
@@ -1620,7 +1635,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="193839872"/>
+        <c:crossAx val="119149696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1633,7 +1648,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600"/>
+            <a:defRPr sz="1800"/>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
         </a:p>
@@ -1643,7 +1658,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1671,6 +1686,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln cmpd="dbl">
+              <a:prstDash val="dash"/>
+            </a:ln>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -1728,6 +1748,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:prstDash val="sysDash"/>
+            </a:ln>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -1785,6 +1810,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:prstDash val="sysDot"/>
+            </a:ln>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -1887,11 +1917,11 @@
         </c:ser>
         <c:dropLines/>
         <c:marker val="1"/>
-        <c:axId val="193903616"/>
-        <c:axId val="193909888"/>
+        <c:axId val="119236480"/>
+        <c:axId val="119246848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="193903616"/>
+        <c:axId val="119236480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1918,14 +1948,14 @@
         </c:title>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="193909888"/>
+        <c:crossAx val="119246848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="193909888"/>
+        <c:axId val="119246848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.3"/>
@@ -1958,7 +1988,7 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="1.6278209396966337E-2"/>
+              <c:x val="1.627820939696634E-2"/>
               <c:y val="0.28633457276173818"/>
             </c:manualLayout>
           </c:layout>
@@ -1975,7 +2005,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="193903616"/>
+        <c:crossAx val="119236480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1988,7 +2018,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600"/>
+            <a:defRPr sz="1800"/>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
         </a:p>
@@ -1998,7 +2028,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2081,13 +2111,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -56843,8 +56873,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="I61" sqref="I61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>